<commit_message>
new gart check type
</commit_message>
<xml_diff>
--- a/errors.xlsx
+++ b/errors.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="93">
   <si>
     <t>RentalAgreementID</t>
   </si>
@@ -46,6 +46,12 @@
     <t>GART FIX</t>
   </si>
   <si>
+    <t>the guest reported leaking and  overheating</t>
+  </si>
+  <si>
+    <t>Turned the windshield wiper on the golf cart and it fell off</t>
+  </si>
+  <si>
     <t>Guest messaged me this morning and let me know that when they were using the home's golf cart / LSV last night, it started smoking. They have it parked at the home and have requested for someone to look at it as soon as possible today.</t>
   </si>
   <si>
@@ -58,6 +64,9 @@
     <t>BIKE CHECK</t>
   </si>
   <si>
+    <t>FIX</t>
+  </si>
+  <si>
     <t>BIKE FIX</t>
   </si>
   <si>
@@ -67,43 +76,169 @@
     <t>ITEM MOVE</t>
   </si>
   <si>
-    <t>AT2: Complete bike check
-AT1:Guest are using 2 bikes</t>
+    <t>QUANTITY CHECK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT2: Complete bike check
+AT1:only one bike on site locked through tire on driveway. guests on site probably using. locks 0021 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT2: Complete bike check, please bring 4 vacayzen taxis
+AT1:No bikes on site </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peloton needs set up, it is not showing an account.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">one of the chains fell off one of the house bikes </t>
+  </si>
+  <si>
+    <t>Please fix loose chain on Exclusive TAXI HB "In Your Dreams" - guest said chain keeps falling off. bike placed on the gravel next to the driveway and side door</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guest reported that the crank on one the bike is broken and on the next bike the chain guard is rubbing against the chain, guest stated that the two bikes are parked next to trash can. Exclusive bikes
+</t>
+  </si>
+  <si>
+    <t>D/o
+(1) Yellow 360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all bikes need air in the tires </t>
+  </si>
+  <si>
+    <t>remove 7 bikes from garage and lock to the bike rack located to the   northeastern section of the property.</t>
+  </si>
+  <si>
+    <t>locate 2 blue on blue 360s and ensure are gtg, bring 2 just in case
+per check: 3/5 blue on blue 360s locked through tires on bike rack by boardwalk. locks 0121 labeled blue door cottage. guests state they called yesterday saying that two bikes have come and gone since they've been here and someone must have their code</t>
+  </si>
+  <si>
+    <t>At2: please complete bike check
+At1: Not onsite</t>
+  </si>
+  <si>
+    <t>Peloton needs set up, it is not showing an account.</t>
+  </si>
+  <si>
+    <t>per exclusive- One bike is missing the little turn knob that adjust the seat. It's on top of the seat and the other Bikes chain is off. Please come service these bikes we have a guest coming in today.</t>
+  </si>
+  <si>
+    <t>per exclusive- One of the bike chain fall off. Please tighten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activate peloton, it got deactivated </t>
+  </si>
+  <si>
+    <t xml:space="preserve">per guest "  one that has an issue with the pedal and another that chain keeps coming off if they could check that one as well that would be great please! We are headed out for a little while but the bikes are under the carport!" </t>
+  </si>
+  <si>
+    <t>AT2: Complete bike check, yellow 360s
+AT1:4/6 bikes at property (2 being used) All bikes at property are good - checked locks, labels, and tire pressure.</t>
+  </si>
+  <si>
+    <t>Guest is reporting a house bike has a flat tire.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1) house bike missing, please ensure all bikes onsite if not, d/o 1 yellow 360 and also pick up 2 rental bikes from this property </t>
+  </si>
+  <si>
+    <t>Please make sure bikes are located on a bike rack near building 46. Sent photo to logistics</t>
+  </si>
+  <si>
+    <t>Swap one white blue tire with popped tube.</t>
+  </si>
+  <si>
+    <t>Please cut and replace lock, set code to attributes
+Per check: Bike condition good. 
+Bike on right has jammed lock or incorrect code. Unable to crack it. Needs to be cut or cracked and reset</t>
+  </si>
+  <si>
+    <t>there are possibly (3) HB here 65 vista bluffs that belong at 84 Pompano Street. "Dot worry beach happy" please take them back to the property -84 Pompano Street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT2: Complete bike check
+AT1:Guest are using 2 bikes </t>
   </si>
   <si>
     <t>AT2: Complete bike check
 AT1:Guest using 3 bikes</t>
   </si>
   <si>
+    <t>AT2: Complete bike check, bring 2 exclusives
+AT1:2 bikes not on site. Guest are home</t>
+  </si>
+  <si>
     <t>AT2: Complete bike check
 AT1:No bike on site. Guest are inside</t>
   </si>
   <si>
-    <t>Homeowner would like help getting the back nutt off so they can attach their own burley.</t>
+    <t xml:space="preserve">Homeowner would like help getting the back nutt off so they can attach their own burley. </t>
   </si>
   <si>
     <t>D/o
 (1) Exclusive 30a</t>
   </si>
   <si>
-    <t>Item Move/Bike Fix
-the guest left a bike on a bike rack across from the property by the bike shop they have it locked up and they told us that the code for the lock is not working so they cannot put the bike back in the garage before they leave so it needs to be returned to the property.</t>
+    <t xml:space="preserve">Item Move/Bike Fix
+the guest left a bike on a bike rack across from the property by the bike shop they have it locked up and they told us that the code for the lock is not working so they cannot put the bike back in the garage before they leave so it needs to be returned to the property. </t>
   </si>
   <si>
     <t>PM reported one of them has no air and another has a seat loose</t>
   </si>
   <si>
-    <t>Item Move // Fix
-she was riding on 30A the chain broke it is located on the beachside of 30A between Alys Beach and Prominence and needs to be picked up and returned back to the home. Trying to get more info on where it was placed!</t>
+    <t xml:space="preserve">Item Move // Fix
+she was riding on 30A the chain broke it is located on the beachside of 30A between Alys Beach and Prominence and needs to be picked up and returned back to the home. Trying to get more info on where it was placed! </t>
   </si>
   <si>
     <t>PICKUP</t>
   </si>
   <si>
-    <t>Guest reported that the chain on the 24" bike keeps falling off and is not staying on.  Please tighten.</t>
-  </si>
-  <si>
-    <t>bike locks are jammed guests are unable to unlock bikes</t>
+    <t>DELIVERY ONLY</t>
+  </si>
+  <si>
+    <t>Please replace chain on (1) 24" and (1) 20" bike. Please reset lock on 16" bike. Guest reported chain issues and a bike lock that will open. The bikes will be back to the house after 4pm.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT2: Pick up (1) 26" rental. Guest extended
+AT1: bike was not on site when I went by.  </t>
+  </si>
+  <si>
+    <t>AT2: Pick up (4) 26" rentals</t>
+  </si>
+  <si>
+    <t>Please pump up tires in (1) 16" bike</t>
+  </si>
+  <si>
+    <t>Please pump up tires on (1) 24" bike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code 5907 is not working -please ensure the lock code is working </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT3: Pick up (1) 20' rental guest put outside last night
+AT2: Bike is still not on site  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">D/O Guest is missing 1 backpack beach chair. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1) 26" bike has a popped tube and wants to have the bike swapped, the guest also stated that he is about 6 miles away from his rental address, 147 West La Garza in Alys Beach. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT2: pick up (1) infant crib sheet from kitchen counter. Cleaners picked it up accidentally
+AT1: Picked up crib there was no sheet though   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please deliver (2) double jogging strollers
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guest reported that the chain on the 24" bike keeps falling off and is not staying on.  Please tighten. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bike locks are jammed guests are unable to unlock bikes </t>
   </si>
   <si>
     <t>AT2: pick up (4) 26: rentals
@@ -114,12 +249,12 @@
 AT1: **picked up 3/4 26in bikes**</t>
   </si>
   <si>
-    <t>AT2: pick up (1) 20" rental
-AT1: Not on site</t>
-  </si>
-  <si>
-    <t>AT2: Pick up (1) 20" rental
-AT1: One of the 20 inch bikes is not on site</t>
+    <t xml:space="preserve">AT2: pick up (1) 20" rental
+AT1: Not on site </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT2: Pick up (1) 20" rental
+AT1: One of the 20 inch bikes is not on site </t>
   </si>
   <si>
     <t>AT2: Pick up (1) 26" w/baby seat, (1) adult helmet, (1) kid  helmet, (3) bp beach chairs, (2) 20" rentals, and (2) youth helmets.
@@ -138,16 +273,16 @@
 AT1: could not locate bike on site, bike was picked up from seagrove store. told to star for time being</t>
   </si>
   <si>
-    <t>AT2: Pick up (1) KT
-AT1: 24 on site , no sign of KT</t>
-  </si>
-  <si>
-    <t>AT2: Pick up (1) 26" rental.
-AT1: 24” picked up, 26” not on site , seat on 24” loose/broken on arrival</t>
-  </si>
-  <si>
-    <t>AT2: Pick up (1) 26" rental and (1) KT
-AT1: 26 and KT not here</t>
+    <t xml:space="preserve">AT2: Pick up (1) KT
+AT1: 24 on site , no sign of KT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT2: Pick up (1) 26" rental.
+AT1: 24” picked up, 26” not on site , seat on 24” loose/broken on arrival  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT2: Pick up (1) 26" rental and (1) KT
+AT1: 26 and KT not here  </t>
   </si>
   <si>
     <t>AT2: Pick up (3) 26" rentals. Guest extended after pick up attempt
@@ -169,7 +304,7 @@
 AT2: locate and pick up (2) 26" bikes.</t>
   </si>
   <si>
-    <t>1 (26") seat is broke and can not ride on</t>
+    <t xml:space="preserve">1 (26") seat is broke and can not ride on </t>
   </si>
   <si>
     <t>ID</t>
@@ -558,7 +693,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -592,10 +727,10 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
-        <v>36046</v>
+        <v>55606</v>
       </c>
       <c r="B2" s="2">
-        <v>45366</v>
+        <v>45368</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -615,16 +750,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
-        <v>25863</v>
+        <v>55606</v>
       </c>
       <c r="B3" s="2">
-        <v>45364</v>
+        <v>45368</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -638,24 +773,93 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
-        <v>918</v>
+        <v>47177</v>
       </c>
       <c r="B4" s="2">
-        <v>45364</v>
+        <v>45368</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>36046</v>
+      </c>
+      <c r="B5" s="2">
+        <v>45366</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" t="b">
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>25863</v>
+      </c>
+      <c r="B6" s="2">
+        <v>45364</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>918</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45364</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="b">
         <v>1</v>
       </c>
     </row>
@@ -666,7 +870,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -700,16 +904,16 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
-        <v>57571</v>
+        <v>67781</v>
       </c>
       <c r="B2" s="2">
-        <v>45366</v>
+        <v>45368</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -723,16 +927,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
-        <v>51628</v>
+        <v>67324</v>
       </c>
       <c r="B3" s="2">
-        <v>45366</v>
+        <v>45368</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -746,22 +950,22 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
-        <v>9379</v>
+        <v>59619</v>
       </c>
       <c r="B4" s="2">
-        <v>45366</v>
+        <v>45368</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" t="b">
         <v>1</v>
@@ -769,22 +973,22 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5">
-        <v>6008</v>
+        <v>29706</v>
       </c>
       <c r="B5" s="2">
-        <v>45366</v>
+        <v>45368</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="b">
         <v>1</v>
@@ -792,16 +996,16 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6">
-        <v>1036</v>
+        <v>9375</v>
       </c>
       <c r="B6" s="2">
-        <v>45366</v>
+        <v>45368</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -815,16 +1019,16 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7">
-        <v>67149</v>
+        <v>6013</v>
       </c>
       <c r="B7" s="2">
-        <v>45365</v>
+        <v>45368</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -838,16 +1042,16 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8">
-        <v>51094</v>
+        <v>1329</v>
       </c>
       <c r="B8" s="2">
-        <v>45365</v>
+        <v>45368</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -861,16 +1065,16 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9">
-        <v>38146</v>
+        <v>1070</v>
       </c>
       <c r="B9" s="2">
-        <v>45365</v>
+        <v>45368</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -884,24 +1088,576 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10">
+        <v>988</v>
+      </c>
+      <c r="B10" s="2">
+        <v>45368</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11">
+        <v>971</v>
+      </c>
+      <c r="B11" s="2">
+        <v>45368</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>67324</v>
+      </c>
+      <c r="B12" s="2">
+        <v>45367</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>59619</v>
+      </c>
+      <c r="B13" s="2">
+        <v>45367</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <v>30170</v>
+      </c>
+      <c r="B14" s="2">
+        <v>45367</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <v>30170</v>
+      </c>
+      <c r="B15" s="2">
+        <v>45367</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>30166</v>
+      </c>
+      <c r="B16" s="2">
+        <v>45367</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>29706</v>
+      </c>
+      <c r="B17" s="2">
+        <v>45367</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>1344</v>
+      </c>
+      <c r="B18" s="2">
+        <v>45367</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>1329</v>
+      </c>
+      <c r="B19" s="2">
+        <v>45367</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>1328</v>
+      </c>
+      <c r="B20" s="2">
+        <v>45367</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>1292</v>
+      </c>
+      <c r="B21" s="2">
+        <v>45367</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <v>1240</v>
+      </c>
+      <c r="B22" s="2">
+        <v>45367</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <v>1128</v>
+      </c>
+      <c r="B23" s="2">
+        <v>45367</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>897</v>
+      </c>
+      <c r="B24" s="2">
+        <v>45367</v>
+      </c>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>57571</v>
+      </c>
+      <c r="B25" s="2">
+        <v>45366</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26">
+        <v>51628</v>
+      </c>
+      <c r="B26" s="2">
+        <v>45366</v>
+      </c>
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27">
+        <v>9379</v>
+      </c>
+      <c r="B27" s="2">
+        <v>45366</v>
+      </c>
+      <c r="C27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28">
+        <v>6047</v>
+      </c>
+      <c r="B28" s="2">
+        <v>45366</v>
+      </c>
+      <c r="C28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" t="b">
+        <v>0</v>
+      </c>
+      <c r="H28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29">
+        <v>6008</v>
+      </c>
+      <c r="B29" s="2">
+        <v>45366</v>
+      </c>
+      <c r="C29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30">
+        <v>1036</v>
+      </c>
+      <c r="B30" s="2">
+        <v>45366</v>
+      </c>
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
+        <v>67149</v>
+      </c>
+      <c r="B31" s="2">
+        <v>45365</v>
+      </c>
+      <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" t="s">
+        <v>48</v>
+      </c>
+      <c r="F31" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32">
+        <v>51094</v>
+      </c>
+      <c r="B32" s="2">
+        <v>45365</v>
+      </c>
+      <c r="C32" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" t="s">
+        <v>49</v>
+      </c>
+      <c r="F32" t="b">
+        <v>0</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33">
         <v>38146</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B33" s="2">
         <v>45365</v>
       </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G10" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" t="b">
+      <c r="C33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34">
+        <v>38146</v>
+      </c>
+      <c r="B34" s="2">
+        <v>45365</v>
+      </c>
+      <c r="C34" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" t="s">
+        <v>51</v>
+      </c>
+      <c r="F34" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" t="b">
         <v>1</v>
       </c>
     </row>
@@ -912,7 +1668,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -946,16 +1702,16 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
-        <v>70367</v>
+        <v>70404</v>
       </c>
       <c r="B2" s="2">
-        <v>45366</v>
+        <v>45368</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -969,22 +1725,22 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
-        <v>70322</v>
+        <v>70260</v>
       </c>
       <c r="B3" s="2">
-        <v>45366</v>
+        <v>45368</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="F3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" t="b">
         <v>1</v>
@@ -992,16 +1748,16 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
-        <v>70289</v>
+        <v>70121</v>
       </c>
       <c r="B4" s="2">
-        <v>45366</v>
+        <v>45368</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -1015,22 +1771,22 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5">
-        <v>70163</v>
+        <v>69261</v>
       </c>
       <c r="B5" s="2">
-        <v>45366</v>
+        <v>45368</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="F5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="b">
         <v>1</v>
@@ -1038,22 +1794,22 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6">
-        <v>70135</v>
+        <v>69258</v>
       </c>
       <c r="B6" s="2">
-        <v>45366</v>
+        <v>45368</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="F6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="b">
         <v>1</v>
@@ -1061,22 +1817,22 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7">
-        <v>69854</v>
+        <v>69172</v>
       </c>
       <c r="B7" s="2">
-        <v>45366</v>
+        <v>45368</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="F7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="b">
         <v>1</v>
@@ -1084,16 +1840,16 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8">
-        <v>69779</v>
+        <v>70135</v>
       </c>
       <c r="B8" s="2">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
@@ -1107,22 +1863,22 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9">
-        <v>69555</v>
+        <v>69825</v>
       </c>
       <c r="B9" s="2">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="F9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" t="b">
         <v>1</v>
@@ -1130,22 +1886,22 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10">
-        <v>68906</v>
+        <v>69815</v>
       </c>
       <c r="B10" s="2">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="F10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="b">
         <v>1</v>
@@ -1153,16 +1909,16 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11">
-        <v>70225</v>
+        <v>69585</v>
       </c>
       <c r="B11" s="2">
-        <v>45365</v>
+        <v>45367</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
@@ -1176,22 +1932,22 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12">
-        <v>70100</v>
+        <v>69293</v>
       </c>
       <c r="B12" s="2">
-        <v>45365</v>
+        <v>45367</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="F12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="b">
         <v>1</v>
@@ -1199,22 +1955,22 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13">
-        <v>70099</v>
+        <v>70367</v>
       </c>
       <c r="B13" s="2">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="F13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="b">
         <v>1</v>
@@ -1222,22 +1978,22 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14">
-        <v>70092</v>
+        <v>70322</v>
       </c>
       <c r="B14" s="2">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="F14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="b">
         <v>1</v>
@@ -1245,16 +2001,16 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15">
-        <v>69992</v>
+        <v>70289</v>
       </c>
       <c r="B15" s="2">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="F15" t="b">
         <v>1</v>
@@ -1268,22 +2024,22 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16">
-        <v>69915</v>
+        <v>70163</v>
       </c>
       <c r="B16" s="2">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="F16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" t="b">
         <v>1</v>
@@ -1291,16 +2047,16 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17">
-        <v>69824</v>
+        <v>70135</v>
       </c>
       <c r="B17" s="2">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="E17" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="F17" t="b">
         <v>1</v>
@@ -1314,16 +2070,16 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18">
-        <v>69533</v>
+        <v>69854</v>
       </c>
       <c r="B18" s="2">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="E18" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="F18" t="b">
         <v>1</v>
@@ -1337,16 +2093,16 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19">
-        <v>69710</v>
+        <v>69779</v>
       </c>
       <c r="B19" s="2">
-        <v>45364</v>
+        <v>45366</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="F19" t="b">
         <v>1</v>
@@ -1360,24 +2116,277 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20">
+        <v>69555</v>
+      </c>
+      <c r="B20" s="2">
+        <v>45366</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>68906</v>
+      </c>
+      <c r="B21" s="2">
+        <v>45366</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <v>70225</v>
+      </c>
+      <c r="B22" s="2">
+        <v>45365</v>
+      </c>
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <v>70100</v>
+      </c>
+      <c r="B23" s="2">
+        <v>45365</v>
+      </c>
+      <c r="C23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>70099</v>
+      </c>
+      <c r="B24" s="2">
+        <v>45365</v>
+      </c>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>70092</v>
+      </c>
+      <c r="B25" s="2">
+        <v>45365</v>
+      </c>
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" t="s">
+        <v>77</v>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26">
+        <v>69992</v>
+      </c>
+      <c r="B26" s="2">
+        <v>45365</v>
+      </c>
+      <c r="C26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" t="s">
+        <v>78</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27">
+        <v>69915</v>
+      </c>
+      <c r="B27" s="2">
+        <v>45365</v>
+      </c>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28">
+        <v>69824</v>
+      </c>
+      <c r="B28" s="2">
+        <v>45365</v>
+      </c>
+      <c r="C28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" t="s">
+        <v>80</v>
+      </c>
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" t="b">
+        <v>0</v>
+      </c>
+      <c r="H28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29">
+        <v>69533</v>
+      </c>
+      <c r="B29" s="2">
+        <v>45365</v>
+      </c>
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" t="s">
+        <v>81</v>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30">
+        <v>69710</v>
+      </c>
+      <c r="B30" s="2">
+        <v>45364</v>
+      </c>
+      <c r="C30" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
         <v>69686</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B31" s="2">
         <v>45364</v>
       </c>
-      <c r="C20" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" t="b">
-        <v>0</v>
-      </c>
-      <c r="G20" t="b">
-        <v>1</v>
-      </c>
-      <c r="H20" t="b">
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1396,34 +2405,34 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>52</v>
+        <v>92</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>7</v>

</xml_diff>